<commit_message>
Minor plot display updates
</commit_message>
<xml_diff>
--- a/Code/method comparison.xlsx
+++ b/Code/method comparison.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livemanchesterac-my.sharepoint.com/personal/neil_power-2_student_manchester_ac_uk/Documents/Physics/Year 4/MoonPhys/mphys-moon/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DC5CE5DC-6B86-43DE-A1C5-7CC76CD44403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{DC5CE5DC-6B86-43DE-A1C5-7CC76CD44403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0E79E85-D626-4402-9388-0DFB9FAF987A}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="method comparison" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -94,9 +107,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -578,7 +591,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -934,22 +947,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.9296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.3984375" customWidth="1"/>
-    <col min="16" max="19" width="12.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="16" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -984,319 +997,319 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.92007743362831795</v>
-      </c>
-      <c r="D2" s="1">
-        <v>7.3031891644116699E-3</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.97333163881509699</v>
-      </c>
-      <c r="F2" s="1">
-        <v>3.68858215799022E-3</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0.89497645713770202</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1.2459036105631901E-2</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.92297718481034097</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1.32245818357845E-2</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0.908658443825615</v>
-      </c>
-      <c r="L2" s="1">
-        <v>8.3948881058608493E-3</v>
+      <c r="C2">
+        <v>0.92228982300884899</v>
+      </c>
+      <c r="D2">
+        <v>7.8522293319812607E-3</v>
+      </c>
+      <c r="E2">
+        <v>0.97469315859757999</v>
+      </c>
+      <c r="F2">
+        <v>3.9706671054685096E-3</v>
+      </c>
+      <c r="G2">
+        <v>0.89917198838871304</v>
+      </c>
+      <c r="H2">
+        <v>1.50722697451505E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.92615721526494099</v>
+      </c>
+      <c r="J2">
+        <v>1.47247588875365E-2</v>
+      </c>
+      <c r="K2">
+        <v>0.91230919082180495</v>
+      </c>
+      <c r="L2">
+        <v>9.0701829593114094E-3</v>
       </c>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.91178097345132703</v>
-      </c>
-      <c r="D3" s="1">
-        <v>8.0750318198174395E-3</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.96807906685719902</v>
-      </c>
-      <c r="F3" s="1">
-        <v>4.3925649741743296E-3</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.88732712741651099</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1.2438351199630601E-2</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.91544483961669199</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1.1594584159715701E-2</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0.90110679173614605</v>
-      </c>
-      <c r="L3" s="1">
-        <v>9.5613143817463997E-3</v>
+      <c r="C3">
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="D3">
+        <v>8.6531014630993105E-3</v>
+      </c>
+      <c r="E3">
+        <v>0.96881585228144995</v>
+      </c>
+      <c r="F3">
+        <v>5.0931002999141904E-3</v>
+      </c>
+      <c r="G3">
+        <v>0.88693416327011299</v>
+      </c>
+      <c r="H3">
+        <v>1.4816604246453599E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.91475960335281103</v>
+      </c>
+      <c r="J3">
+        <v>1.23283408584579E-2</v>
+      </c>
+      <c r="K3">
+        <v>0.90053396226914995</v>
+      </c>
+      <c r="L3">
+        <v>1.001378553969E-2</v>
       </c>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.88987831858406996</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1.0647518956008101E-2</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.88884558733941699</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1.08972615244704E-2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.88074902147173195</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1.3638327887527901E-2</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0.86995754163607497</v>
-      </c>
-      <c r="J4" s="1">
-        <v>1.8450846910078401E-2</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0.87519522280366702</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1.24878786862904E-2</v>
+      <c r="C4">
+        <v>0.88971238938053099</v>
+      </c>
+      <c r="D4">
+        <v>9.2093614586461203E-3</v>
+      </c>
+      <c r="E4">
+        <v>0.88827718521503096</v>
+      </c>
+      <c r="F4">
+        <v>9.5362346888544797E-3</v>
+      </c>
+      <c r="G4">
+        <v>0.87844221649689702</v>
+      </c>
+      <c r="H4">
+        <v>2.1863716537628801E-2</v>
+      </c>
+      <c r="I4">
+        <v>0.86619506891888898</v>
+      </c>
+      <c r="J4">
+        <v>1.72418587933654E-2</v>
+      </c>
+      <c r="K4">
+        <v>0.87198335763132995</v>
+      </c>
+      <c r="L4">
+        <v>1.1486463821347799E-2</v>
       </c>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.80193584070796398</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1.25223730782924E-2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.88269090679028706</v>
-      </c>
-      <c r="F5" s="1">
-        <v>9.9045139318486592E-3</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.77330431672711397</v>
-      </c>
-      <c r="H5" s="1">
-        <v>2.0470331978247502E-2</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.76718717065896702</v>
-      </c>
-      <c r="J5" s="1">
-        <v>1.89444361076022E-2</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0.77006759335921404</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1.6298778266303601E-2</v>
+      <c r="C5">
+        <v>0.88213495575221201</v>
+      </c>
+      <c r="D5">
+        <v>1.1792652817188901E-2</v>
+      </c>
+      <c r="E5">
+        <v>0.94441582524317802</v>
+      </c>
+      <c r="F5">
+        <v>7.9530702922134995E-3</v>
+      </c>
+      <c r="G5">
+        <v>0.85192894578397704</v>
+      </c>
+      <c r="H5">
+        <v>1.8402467979269199E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.884161832701991</v>
+      </c>
+      <c r="J5">
+        <v>1.71116276412259E-2</v>
+      </c>
+      <c r="K5">
+        <v>0.86758553844462505</v>
+      </c>
+      <c r="L5">
+        <v>1.34749866429776E-2</v>
       </c>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1">
-        <v>0.827599557522123</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1.1277083852353599E-2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.92060256986474698</v>
-      </c>
-      <c r="F6" s="1">
-        <v>9.1597144176754595E-3</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.86158127956036401</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1.6326716154870101E-2</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.72123050322748405</v>
-      </c>
-      <c r="J6" s="1">
-        <v>2.4055141129003001E-2</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0.78494029682617605</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1.68335239604804E-2</v>
+      <c r="C6">
+        <v>0.84789823008849496</v>
+      </c>
+      <c r="D6">
+        <v>7.52293722828288E-3</v>
+      </c>
+      <c r="E6">
+        <v>0.920003446209121</v>
+      </c>
+      <c r="F6">
+        <v>4.9862061724843696E-3</v>
+      </c>
+      <c r="G6">
+        <v>0.85995306951300798</v>
+      </c>
+      <c r="H6">
+        <v>1.1909195426786701E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.78170764724566</v>
+      </c>
+      <c r="J6">
+        <v>1.43494541724472E-2</v>
+      </c>
+      <c r="K6">
+        <v>0.81886839084595298</v>
+      </c>
+      <c r="L6">
+        <v>1.0089237597172999E-2</v>
       </c>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1">
-        <v>0.90215707964601699</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.07675141036997E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.96067284302440303</v>
-      </c>
-      <c r="F7" s="1">
-        <v>7.1338120360505998E-3</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.88653168165500296</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1.2316847800643699E-2</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.89142847862494001</v>
-      </c>
-      <c r="J7" s="1">
-        <v>1.70339285105881E-2</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0.88890053482434495</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1.2490547327875899E-2</v>
+      <c r="C7">
+        <v>0.90094026548672501</v>
+      </c>
+      <c r="D7">
+        <v>9.6020948825558394E-3</v>
+      </c>
+      <c r="E7">
+        <v>0.96146874641498004</v>
+      </c>
+      <c r="F7">
+        <v>5.9980239178495801E-3</v>
+      </c>
+      <c r="G7">
+        <v>0.88192423881016702</v>
+      </c>
+      <c r="H7">
+        <v>1.8375229555915799E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.89268097296339599</v>
+      </c>
+      <c r="J7">
+        <v>1.9235152753396299E-2</v>
+      </c>
+      <c r="K7">
+        <v>0.887045371822335</v>
+      </c>
+      <c r="L7">
+        <v>1.24628301196515E-2</v>
       </c>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1">
-        <v>0.79629424778761004</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1.14333395655885E-2</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.82752345363461799</v>
-      </c>
-      <c r="F8" s="1">
-        <v>9.9935837284988692E-3</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.85635828970392402</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2.00878551651823E-2</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.64594100969124402</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1.85907909390092E-2</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0.73621346685014899</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1.54752251663949E-2</v>
+      <c r="C8">
+        <v>0.882411504424778</v>
+      </c>
+      <c r="D8">
+        <v>9.2821534052204297E-3</v>
+      </c>
+      <c r="E8">
+        <v>0.88825468937131202</v>
+      </c>
+      <c r="F8">
+        <v>8.4226285403778099E-3</v>
+      </c>
+      <c r="G8">
+        <v>0.86949473774049102</v>
+      </c>
+      <c r="H8">
+        <v>1.7718782598762198E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.85951028898346504</v>
+      </c>
+      <c r="J8">
+        <v>1.7339382279040999E-2</v>
+      </c>
+      <c r="K8">
+        <v>0.86427720641071004</v>
+      </c>
+      <c r="L8">
+        <v>1.1657419361581199E-2</v>
       </c>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1">
-        <v>0.91028761061946895</v>
-      </c>
-      <c r="D9" s="1">
-        <v>6.4492194013931001E-3</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.96654609193984897</v>
-      </c>
-      <c r="F9" s="1">
-        <v>5.3280831533568697E-3</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.88976752830016004</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1.5472372427085899E-2</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0.90628701019747004</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1.32240188601479E-2</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0.897812087714705</v>
-      </c>
-      <c r="L9" s="1">
-        <v>9.2263748293274495E-3</v>
+      <c r="C9">
+        <v>0.90918141592920299</v>
+      </c>
+      <c r="D9">
+        <v>7.9376695579248709E-3</v>
+      </c>
+      <c r="E9">
+        <v>0.96553470236188799</v>
+      </c>
+      <c r="F9">
+        <v>5.5578850064962699E-3</v>
+      </c>
+      <c r="G9">
+        <v>0.88608076599904995</v>
+      </c>
+      <c r="H9">
+        <v>1.6771690378891101E-2</v>
+      </c>
+      <c r="I9">
+        <v>0.91178378817732497</v>
+      </c>
+      <c r="J9">
+        <v>1.4968306600630201E-2</v>
+      </c>
+      <c r="K9">
+        <v>0.89856256225253694</v>
+      </c>
+      <c r="L9">
+        <v>9.3421390452220303E-3</v>
       </c>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -1335,7 +1348,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -1370,7 +1383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N12" t="str">
         <f>B1</f>
         <v>Method</v>
@@ -1391,21 +1404,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="1">
         <f>ROUND(C2,3)</f>
-        <v>0.92</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" ref="D13:L13" si="0">ROUND(D2,3)</f>
-        <v>7.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0.97299999999999998</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
@@ -1413,27 +1426,27 @@
       </c>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
-        <v>0.89500000000000002</v>
+        <v>0.89900000000000002</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="0"/>
-        <v>1.2E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>0.92300000000000004</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="0"/>
-        <v>1.2999999999999999E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K13" s="1">
         <f t="shared" si="0"/>
-        <v>0.90900000000000003</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="0"/>
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1" t="str">
@@ -1442,41 +1455,41 @@
       </c>
       <c r="O13" t="str">
         <f>_xlfn.CONCAT(C13&amp;REPT("0",5-LEN(C13))," ± ",D13&amp;REPT("0",5-LEN(D13)))</f>
-        <v>0.920 ± 0.007</v>
+        <v>0.922 ± 0.008</v>
       </c>
       <c r="P13" t="str">
         <f>_xlfn.CONCAT(E13&amp;REPT("0",5-LEN(E13))," ± ",F13&amp;REPT("0",5-LEN(F13)))</f>
-        <v>0.973 ± 0.004</v>
+        <v>0.975 ± 0.004</v>
       </c>
       <c r="Q13" t="str">
         <f>_xlfn.CONCAT(G13&amp;REPT("0",5-LEN(G13))," ± ",H13&amp;REPT("0",5-LEN(H13)))</f>
-        <v>0.895 ± 0.012</v>
+        <v>0.899 ± 0.015</v>
       </c>
       <c r="R13" t="str">
         <f>_xlfn.CONCAT(I13&amp;REPT("0",5-LEN(I13))," ± ",J13&amp;REPT("0",5-LEN(J13)))</f>
-        <v>0.923 ± 0.013</v>
+        <v>0.926 ± 0.015</v>
       </c>
       <c r="S13" t="str">
         <f>_xlfn.CONCAT(K13&amp;REPT("0",5-LEN(K13))," ± ",L13&amp;REPT("0",5-LEN(L13)))</f>
-        <v>0.909 ± 0.008</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+        <v>0.912 ± 0.009</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <f t="shared" ref="C14:L20" si="1">ROUND(C3,3)</f>
-        <v>0.91200000000000003</v>
+        <v>0.91300000000000003</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="1"/>
-        <v>0.96799999999999997</v>
+        <v>0.96899999999999997</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="1"/>
-        <v>4.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
@@ -1484,7 +1497,7 @@
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="1"/>
@@ -1509,15 +1522,15 @@
       </c>
       <c r="O14" t="str">
         <f t="shared" ref="O14:O20" si="3">_xlfn.CONCAT(C14&amp;REPT("0",5-LEN(C14))," ± ",D14&amp;REPT("0",5-LEN(D14)))</f>
-        <v>0.912 ± 0.008</v>
+        <v>0.913 ± 0.009</v>
       </c>
       <c r="P14" t="str">
         <f t="shared" ref="P14:P20" si="4">_xlfn.CONCAT(E14&amp;REPT("0",5-LEN(E14))," ± ",F14&amp;REPT("0",5-LEN(F14)))</f>
-        <v>0.968 ± 0.004</v>
+        <v>0.969 ± 0.005</v>
       </c>
       <c r="Q14" t="str">
         <f t="shared" ref="Q14:Q20" si="5">_xlfn.CONCAT(G14&amp;REPT("0",5-LEN(G14))," ± ",H14&amp;REPT("0",5-LEN(H14)))</f>
-        <v>0.887 ± 0.012</v>
+        <v>0.887 ± 0.015</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" ref="R14:R20" si="6">_xlfn.CONCAT(I14&amp;REPT("0",5-LEN(I14))," ± ",J14&amp;REPT("0",5-LEN(J14)))</f>
@@ -1528,46 +1541,46 @@
         <v>0.901 ± 0.010</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <f t="shared" si="1"/>
         <v>0.89</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.878</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.872</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="1"/>
         <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="1"/>
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>0.88100000000000001</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" si="1"/>
-        <v>1.4E-2</v>
-      </c>
-      <c r="I15" s="1">
-        <f t="shared" si="1"/>
-        <v>0.87</v>
-      </c>
-      <c r="J15" s="1">
-        <f t="shared" si="1"/>
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="K15" s="1">
-        <f t="shared" si="1"/>
-        <v>0.875</v>
-      </c>
-      <c r="L15" s="1">
-        <f t="shared" si="1"/>
-        <v>1.2E-2</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1" t="str">
@@ -1576,65 +1589,65 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="3"/>
-        <v>0.890 ± 0.011</v>
+        <v>0.890 ± 0.009</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="4"/>
-        <v>0.889 ± 0.011</v>
+        <v>0.888 ± 0.010</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="5"/>
-        <v>0.881 ± 0.014</v>
+        <v>0.878 ± 0.022</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="6"/>
-        <v>0.870 ± 0.018</v>
+        <v>0.866 ± 0.017</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="7"/>
-        <v>0.875 ± 0.012</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+        <v>0.872 ± 0.011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>0.80200000000000005</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
+        <v>1.2E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="1"/>
         <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.88300000000000001</v>
-      </c>
-      <c r="F16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.77300000000000002</v>
-      </c>
-      <c r="H16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-      <c r="I16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="J16" s="1">
-        <f t="shared" si="1"/>
-        <v>1.9E-2</v>
-      </c>
-      <c r="K16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.77</v>
-      </c>
-      <c r="L16" s="1">
-        <f t="shared" si="1"/>
-        <v>1.6E-2</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1" t="str">
@@ -1643,65 +1656,65 @@
       </c>
       <c r="O16" t="str">
         <f t="shared" si="3"/>
-        <v>0.802 ± 0.013</v>
+        <v>0.882 ± 0.012</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" si="4"/>
-        <v>0.883 ± 0.010</v>
+        <v>0.944 ± 0.008</v>
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="5"/>
-        <v>0.773 ± 0.020</v>
+        <v>0.852 ± 0.018</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" si="6"/>
-        <v>0.767 ± 0.019</v>
+        <v>0.884 ± 0.017</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="7"/>
-        <v>0.770 ± 0.016</v>
-      </c>
-    </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.45">
+        <v>0.868 ± 0.013</v>
+      </c>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>0.82799999999999996</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>1.0999999999999999E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="1"/>
-        <v>0.92100000000000004</v>
+        <v>0.92</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="1"/>
-        <v>8.9999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="1"/>
-        <v>0.86199999999999999</v>
+        <v>0.86</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="1"/>
-        <v>0.72099999999999997</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="1"/>
-        <v>2.4E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="K17" s="1">
         <f t="shared" si="1"/>
-        <v>0.78500000000000003</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="1"/>
-        <v>1.7000000000000001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="str">
@@ -1710,33 +1723,33 @@
       </c>
       <c r="O17" t="str">
         <f t="shared" si="3"/>
-        <v>0.828 ± 0.011</v>
+        <v>0.848 ± 0.008</v>
       </c>
       <c r="P17" t="str">
         <f t="shared" si="4"/>
-        <v>0.921 ± 0.009</v>
+        <v>0.920 ± 0.005</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="5"/>
-        <v>0.862 ± 0.016</v>
+        <v>0.860 ± 0.012</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" si="6"/>
-        <v>0.721 ± 0.024</v>
+        <v>0.782 ± 0.014</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="7"/>
-        <v>0.785 ± 0.017</v>
-      </c>
-    </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.45">
+        <v>0.819 ± 0.010</v>
+      </c>
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <f t="shared" si="1"/>
-        <v>0.90200000000000002</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
-        <v>1.0999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="1"/>
@@ -1744,27 +1757,27 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="1"/>
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9E-2</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="1"/>
         <v>0.88700000000000001</v>
-      </c>
-      <c r="H18" s="1">
-        <f t="shared" si="1"/>
-        <v>1.2E-2</v>
-      </c>
-      <c r="I18" s="1">
-        <f t="shared" si="1"/>
-        <v>0.89100000000000001</v>
-      </c>
-      <c r="J18" s="1">
-        <f t="shared" si="1"/>
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="K18" s="1">
-        <f t="shared" si="1"/>
-        <v>0.88900000000000001</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" si="1"/>
@@ -1777,65 +1790,65 @@
       </c>
       <c r="O18" t="str">
         <f t="shared" si="3"/>
-        <v>0.902 ± 0.011</v>
+        <v>0.901 ± 0.010</v>
       </c>
       <c r="P18" t="str">
         <f t="shared" si="4"/>
-        <v>0.961 ± 0.007</v>
+        <v>0.961 ± 0.006</v>
       </c>
       <c r="Q18" t="str">
         <f t="shared" si="5"/>
-        <v>0.887 ± 0.012</v>
+        <v>0.882 ± 0.018</v>
       </c>
       <c r="R18" t="str">
         <f t="shared" si="6"/>
-        <v>0.891 ± 0.017</v>
+        <v>0.893 ± 0.019</v>
       </c>
       <c r="S18" t="str">
         <f t="shared" si="7"/>
-        <v>0.889 ± 0.012</v>
-      </c>
-    </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.45">
+        <v>0.887 ± 0.012</v>
+      </c>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <f t="shared" si="1"/>
-        <v>0.79600000000000004</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="1"/>
-        <v>1.0999999999999999E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="1"/>
-        <v>0.82799999999999996</v>
+        <v>0.88800000000000001</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="1"/>
-        <v>0.85599999999999998</v>
+        <v>0.86899999999999999</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="1"/>
-        <v>0.64600000000000002</v>
+        <v>0.86</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="1"/>
-        <v>1.9E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="K19" s="1">
         <f t="shared" si="1"/>
-        <v>0.73599999999999999</v>
+        <v>0.86399999999999999</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" si="1"/>
-        <v>1.4999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1" t="str">
@@ -1844,61 +1857,61 @@
       </c>
       <c r="O19" t="str">
         <f t="shared" si="3"/>
-        <v>0.796 ± 0.011</v>
+        <v>0.882 ± 0.009</v>
       </c>
       <c r="P19" t="str">
         <f t="shared" si="4"/>
-        <v>0.828 ± 0.010</v>
+        <v>0.888 ± 0.008</v>
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="5"/>
-        <v>0.856 ± 0.020</v>
+        <v>0.869 ± 0.018</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" si="6"/>
-        <v>0.646 ± 0.019</v>
+        <v>0.860 ± 0.017</v>
       </c>
       <c r="S19" t="str">
         <f t="shared" si="7"/>
-        <v>0.736 ± 0.015</v>
-      </c>
-    </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.45">
+        <v>0.864 ± 0.012</v>
+      </c>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <f t="shared" si="1"/>
-        <v>0.91</v>
+        <v>0.90900000000000003</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="1"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E20" s="1">
-        <f t="shared" si="1"/>
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
       <c r="G20" s="1">
         <f t="shared" si="1"/>
-        <v>0.89</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="1"/>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="1"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I20" s="1">
-        <f t="shared" si="1"/>
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="J20" s="1">
-        <f t="shared" si="1"/>
-        <v>1.2999999999999999E-2</v>
-      </c>
       <c r="K20" s="1">
         <f t="shared" si="1"/>
-        <v>0.89800000000000002</v>
+        <v>0.89900000000000002</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" si="1"/>
@@ -1911,26 +1924,26 @@
       </c>
       <c r="O20" t="str">
         <f t="shared" si="3"/>
-        <v>0.910 ± 0.006</v>
+        <v>0.909 ± 0.008</v>
       </c>
       <c r="P20" t="str">
         <f t="shared" si="4"/>
-        <v>0.967 ± 0.005</v>
+        <v>0.966 ± 0.006</v>
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="5"/>
-        <v>0.890 ± 0.015</v>
+        <v>0.886 ± 0.017</v>
       </c>
       <c r="R20" t="str">
         <f t="shared" si="6"/>
-        <v>0.906 ± 0.013</v>
+        <v>0.912 ± 0.015</v>
       </c>
       <c r="S20" t="str">
         <f t="shared" si="7"/>
-        <v>0.898 ± 0.009</v>
-      </c>
-    </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.45">
+        <v>0.899 ± 0.009</v>
+      </c>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <f t="shared" ref="C21:L21" si="8">ROUND(C10,3)</f>
         <v>0.89</v>
@@ -1996,7 +2009,7 @@
         <v>0.877 ± 0.017</v>
       </c>
     </row>
-    <row r="22" spans="3:19" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <f t="shared" ref="C22:L22" si="14">ROUND(C11,3)</f>
         <v>0.78800000000000003</v>

</xml_diff>